<commit_message>
updated data cleaning with map plots
</commit_message>
<xml_diff>
--- a/data/races_cleaned.xlsx
+++ b/data/races_cleaned.xlsx
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>-29.1228356</v>
+        <v>-38.4966877</v>
       </c>
       <c r="G19" t="n">
-        <v>167.948132251517</v>
+        <v>145.2389168</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
updated cleaning file and races tables
</commit_message>
<xml_diff>
--- a/data/races_cleaned.xlsx
+++ b/data/races_cleaned.xlsx
@@ -445,7 +445,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Chang International Circuit</t>
+          <t>Buriram International Circuit</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -454,10 +454,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2.7601913</v>
+        <v>14.9630569</v>
       </c>
       <c r="G3" t="n">
-        <v>101.736858607147</v>
+        <v>103.085589428401</v>
       </c>
     </row>
     <row r="4">

</xml_diff>